<commit_message>
table fixed now. just need missing citations added to .bib
</commit_message>
<xml_diff>
--- a/Table1.xlsx
+++ b/Table1.xlsx
@@ -1,17 +1,19 @@
 
 <file path=xl/workbook.xml><?xml version="1.0" encoding="utf-8"?>
-<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr6="http://schemas.microsoft.com/office/spreadsheetml/2016/revision6" xmlns:xr10="http://schemas.microsoft.com/office/spreadsheetml/2016/revision10" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" mc:Ignorable="x15 xr xr6 xr10 xr2">
-  <fileVersion appName="xl" lastEdited="7" lowestEdited="6" rupBuild="21001"/>
-  <workbookPr filterPrivacy="1"/>
-  <xr:revisionPtr revIDLastSave="0" documentId="13_ncr:1_{62B9FCD8-3B49-49C4-89D8-E4CAED6E0B45}" xr6:coauthVersionLast="38" xr6:coauthVersionMax="38" xr10:uidLastSave="{00000000-0000-0000-0000-000000000000}"/>
+<workbook xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships">
+  <fileVersion appName="xl" lastEdited="5" lowestEdited="6" rupBuild="28028"/>
+  <workbookPr filterPrivacy="1" autoCompressPictures="0"/>
   <bookViews>
-    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12650" xr2:uid="{00000000-000D-0000-FFFF-FFFF00000000}"/>
+    <workbookView xWindow="0" yWindow="0" windowWidth="22260" windowHeight="12660"/>
   </bookViews>
   <sheets>
     <sheet name="Sheet1" sheetId="1" r:id="rId1"/>
   </sheets>
-  <calcPr calcId="162913"/>
+  <calcPr calcId="140001" concurrentCalc="0"/>
   <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{7523E5D3-25F3-A5E0-1632-64F254C22452}">
+      <mx:ArchID Flags="2"/>
+    </ext>
     <ext xmlns:x15="http://schemas.microsoft.com/office/spreadsheetml/2010/11/main" uri="{140A7094-0E35-4892-8432-C4D2E57EDEB5}">
       <x15:workbookPr chartTrackingRefBase="1"/>
     </ext>
@@ -22,9 +24,6 @@
 <file path=xl/sharedStrings.xml><?xml version="1.0" encoding="utf-8"?>
 <sst xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" count="28" uniqueCount="28">
   <si>
-    <t>Tools</t>
-  </si>
-  <si>
     <t>meta-analysis</t>
   </si>
   <si>
@@ -67,9 +66,6 @@
     <t>[@Castanho2015;@Busch2017]</t>
   </si>
   <si>
-    <t>Example Paper(s)</t>
-  </si>
-  <si>
     <t>[@Lortie2018]</t>
   </si>
   <si>
@@ -104,12 +100,18 @@
   </si>
   <si>
     <t>[@Mergler2007;@Dickman2014]</t>
+  </si>
+  <si>
+    <t>Tool</t>
+  </si>
+  <si>
+    <t>Representative study</t>
   </si>
 </sst>
 </file>
 
 <file path=xl/styles.xml><?xml version="1.0" encoding="utf-8"?>
-<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:x16r2="http://schemas.microsoft.com/office/spreadsheetml/2015/02/main" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" mc:Ignorable="x14ac x16r2 xr">
+<styleSheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <fonts count="1" x14ac:knownFonts="1">
     <font>
       <sz val="11"/>
@@ -201,7 +203,7 @@
     </a:clrScheme>
     <a:fontScheme name="Office">
       <a:majorFont>
-        <a:latin typeface="Calibri Light" panose="020F0302020204030204"/>
+        <a:latin typeface="Calibri Light"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック Light"/>
@@ -236,7 +238,7 @@
         <a:font script="Geor" typeface="Sylfaen"/>
       </a:majorFont>
       <a:minorFont>
-        <a:latin typeface="Calibri" panose="020F0502020204030204"/>
+        <a:latin typeface="Calibri"/>
         <a:ea typeface=""/>
         <a:cs typeface=""/>
         <a:font script="Jpan" typeface="游ゴシック"/>
@@ -413,139 +415,144 @@
   <a:extraClrSchemeLst/>
   <a:extLst>
     <a:ext uri="{05A4C25C-085E-4340-85A3-A5531E510DB2}">
-      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
+      <thm15:themeFamily xmlns:thm15="http://schemas.microsoft.com/office/thememl/2012/main" xmlns="" name="Office Theme" id="{62F939B6-93AF-4DB8-9C6B-D6C7DFDC589F}" vid="{4A3C46E8-61CC-4603-A589-7422A47A8E4A}"/>
     </a:ext>
   </a:extLst>
 </a:theme>
 </file>
 
 <file path=xl/worksheets/sheet1.xml><?xml version="1.0" encoding="utf-8"?>
-<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" xmlns:xr="http://schemas.microsoft.com/office/spreadsheetml/2014/revision" xmlns:xr2="http://schemas.microsoft.com/office/spreadsheetml/2015/revision2" xmlns:xr3="http://schemas.microsoft.com/office/spreadsheetml/2016/revision3" mc:Ignorable="x14ac xr xr2 xr3" xr:uid="{00000000-0001-0000-0000-000000000000}">
+<worksheet xmlns="http://schemas.openxmlformats.org/spreadsheetml/2006/main" xmlns:r="http://schemas.openxmlformats.org/officeDocument/2006/relationships" xmlns:mc="http://schemas.openxmlformats.org/markup-compatibility/2006" xmlns:x14ac="http://schemas.microsoft.com/office/spreadsheetml/2009/9/ac" mc:Ignorable="x14ac">
   <dimension ref="A1:B14"/>
   <sheetViews>
     <sheetView tabSelected="1" workbookViewId="0">
-      <selection activeCell="A17" sqref="A17"/>
+      <selection activeCell="A2" sqref="A2"/>
     </sheetView>
   </sheetViews>
-  <sheetFormatPr defaultRowHeight="14.5" x14ac:dyDescent="0.35"/>
+  <sheetFormatPr baseColWidth="10" defaultColWidth="8.625" defaultRowHeight="15" x14ac:dyDescent="0"/>
   <cols>
-    <col min="1" max="1" width="48.54296875" bestFit="1" customWidth="1"/>
-    <col min="2" max="2" width="42.54296875" bestFit="1" customWidth="1"/>
+    <col min="1" max="1" width="48.5" bestFit="1" customWidth="1"/>
+    <col min="2" max="2" width="42.5" bestFit="1" customWidth="1"/>
   </cols>
   <sheetData>
-    <row r="1" spans="1:2" x14ac:dyDescent="0.35">
+    <row r="1" spans="1:2">
       <c r="A1" t="s">
+        <v>26</v>
+      </c>
+      <c r="B1" t="s">
+        <v>27</v>
+      </c>
+    </row>
+    <row r="2" spans="1:2">
+      <c r="A2" t="s">
         <v>0</v>
       </c>
-      <c r="B1" t="s">
+      <c r="B2" t="s">
+        <v>13</v>
+      </c>
+    </row>
+    <row r="3" spans="1:2">
+      <c r="A3" t="s">
+        <v>1</v>
+      </c>
+      <c r="B3" t="s">
+        <v>14</v>
+      </c>
+    </row>
+    <row r="4" spans="1:2">
+      <c r="A4" t="s">
+        <v>2</v>
+      </c>
+      <c r="B4" t="s">
         <v>15</v>
       </c>
     </row>
-    <row r="2" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A2" t="s">
-        <v>1</v>
-      </c>
-      <c r="B2" t="s">
-        <v>14</v>
-      </c>
-    </row>
-    <row r="3" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A3" t="s">
-        <v>2</v>
-      </c>
-      <c r="B3" t="s">
+    <row r="5" spans="1:2">
+      <c r="A5" t="s">
+        <v>3</v>
+      </c>
+      <c r="B5" t="s">
         <v>16</v>
       </c>
     </row>
-    <row r="4" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A4" t="s">
-        <v>3</v>
-      </c>
-      <c r="B4" t="s">
+    <row r="6" spans="1:2">
+      <c r="A6" t="s">
+        <v>4</v>
+      </c>
+      <c r="B6" t="s">
         <v>17</v>
       </c>
     </row>
-    <row r="5" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A5" t="s">
-        <v>4</v>
-      </c>
-      <c r="B5" t="s">
+    <row r="7" spans="1:2">
+      <c r="A7" t="s">
+        <v>5</v>
+      </c>
+      <c r="B7" t="s">
         <v>18</v>
       </c>
     </row>
-    <row r="6" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A6" t="s">
-        <v>5</v>
-      </c>
-      <c r="B6" t="s">
+    <row r="8" spans="1:2">
+      <c r="A8" t="s">
+        <v>6</v>
+      </c>
+      <c r="B8" t="s">
         <v>19</v>
       </c>
     </row>
-    <row r="7" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A7" t="s">
-        <v>6</v>
-      </c>
-      <c r="B7" t="s">
+    <row r="9" spans="1:2">
+      <c r="A9" t="s">
+        <v>7</v>
+      </c>
+      <c r="B9" t="s">
         <v>20</v>
       </c>
     </row>
-    <row r="8" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A8" t="s">
-        <v>7</v>
-      </c>
-      <c r="B8" t="s">
+    <row r="10" spans="1:2">
+      <c r="A10" t="s">
+        <v>8</v>
+      </c>
+      <c r="B10" t="s">
         <v>21</v>
       </c>
     </row>
-    <row r="9" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A9" t="s">
-        <v>8</v>
-      </c>
-      <c r="B9" t="s">
+    <row r="11" spans="1:2">
+      <c r="A11" t="s">
+        <v>9</v>
+      </c>
+      <c r="B11" t="s">
         <v>22</v>
       </c>
     </row>
-    <row r="10" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A10" t="s">
-        <v>9</v>
-      </c>
-      <c r="B10" t="s">
+    <row r="12" spans="1:2">
+      <c r="A12" t="s">
+        <v>10</v>
+      </c>
+      <c r="B12" t="s">
         <v>23</v>
       </c>
     </row>
-    <row r="11" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A11" t="s">
-        <v>10</v>
-      </c>
-      <c r="B11" t="s">
+    <row r="13" spans="1:2">
+      <c r="A13" t="s">
+        <v>11</v>
+      </c>
+      <c r="B13" t="s">
         <v>24</v>
       </c>
     </row>
-    <row r="12" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A12" t="s">
-        <v>11</v>
-      </c>
-      <c r="B12" t="s">
+    <row r="14" spans="1:2">
+      <c r="A14" t="s">
+        <v>12</v>
+      </c>
+      <c r="B14" t="s">
         <v>25</v>
-      </c>
-    </row>
-    <row r="13" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A13" t="s">
-        <v>12</v>
-      </c>
-      <c r="B13" t="s">
-        <v>26</v>
-      </c>
-    </row>
-    <row r="14" spans="1:2" x14ac:dyDescent="0.35">
-      <c r="A14" t="s">
-        <v>13</v>
-      </c>
-      <c r="B14" t="s">
-        <v>27</v>
       </c>
     </row>
   </sheetData>
   <pageMargins left="0.7" right="0.7" top="0.75" bottom="0.75" header="0.3" footer="0.3"/>
+  <extLst>
+    <ext xmlns:mx="http://schemas.microsoft.com/office/mac/excel/2008/main" uri="{64002731-A6B0-56B0-2670-7721B7C09600}">
+      <mx:PLV Mode="0" OnePage="0" WScale="0"/>
+    </ext>
+  </extLst>
 </worksheet>
 </file>
</xml_diff>